<commit_message>
Added Number and Symbol layers
</commit_message>
<xml_diff>
--- a/qwertigraph/AuxKeyboardDoc.xlsx
+++ b/qwertigraph/AuxKeyboardDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c5400521de505e9/Documents/GitHub/qwertigraphy/qwertigraph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{A3ADF315-14BA-45B9-8535-254D898CD37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B737AEDC-B5D0-486F-9104-5B057A827A72}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{A3ADF315-14BA-45B9-8535-254D898CD37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A27F6BE1-F5E2-4F79-BC0C-EFBE5D3C5C71}"/>
   <bookViews>
     <workbookView xWindow="2010" yWindow="-110" windowWidth="17300" windowHeight="11020" xr2:uid="{A89E2BCF-2433-45D5-B3E5-DA4D75F99EEE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="100">
   <si>
     <t>Numlock</t>
   </si>
@@ -190,13 +190,157 @@
   </si>
   <si>
     <t>{CapLock}</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>f5</t>
+  </si>
+  <si>
+    <t>f9</t>
+  </si>
+  <si>
+    <t>f12</t>
+  </si>
+  <si>
+    <t>f11</t>
+  </si>
+  <si>
+    <t>f10</t>
+  </si>
+  <si>
+    <t>f6</t>
+  </si>
+  <si>
+    <t>f7</t>
+  </si>
+  <si>
+    <t>f8</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Numbers Layer</t>
+  </si>
+  <si>
+    <t>Symbols Layer</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>Symbols</t>
+  </si>
+  <si>
+    <t>{Volume_Up}</t>
+  </si>
+  <si>
+    <t>{Volume_Mute}</t>
+  </si>
+  <si>
+    <t>{Volume_Down}</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,13 +348,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -357,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -373,6 +528,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,248 +851,696 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9796BF0-55BB-4FAC-B6FE-5BB35D58C06B}">
-  <dimension ref="A2:J13"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.08984375" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1">
+      <c r="A1" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+    <row r="2" spans="1:10" ht="15" thickBot="1">
+      <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="4" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="12" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>
       <c r="I5" s="5"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
+    <row r="6" spans="1:10" ht="15" thickBot="1">
+      <c r="A6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1">
+      <c r="B9" s="5"/>
+      <c r="C9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1">
+      <c r="A11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1">
+      <c r="A12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1">
+      <c r="A13" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1">
+      <c r="B15" s="7"/>
+      <c r="C15" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1">
+      <c r="B16" s="3"/>
+      <c r="C16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1">
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1">
+      <c r="B18" s="7"/>
+      <c r="C18" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="B19" s="3"/>
+      <c r="C19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1">
+      <c r="B20" s="5"/>
+      <c r="C20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
+      <c r="F21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1">
+      <c r="A22" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="10"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1">
+      <c r="A24" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" thickBot="1">
+      <c r="B26" s="7"/>
+      <c r="C26" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" thickBot="1">
+      <c r="B27" s="3"/>
+      <c r="C27" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" thickBot="1">
+      <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="B28" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="5"/>
-      <c r="C11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" thickBot="1">
+      <c r="B29" s="7"/>
+      <c r="C29" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30" s="3"/>
+      <c r="C30" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" thickBot="1">
+      <c r="B31" s="5"/>
+      <c r="C31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" thickBot="1">
+      <c r="A32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="12"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
+      <c r="B32" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" thickBot="1">
+      <c r="A33" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="1" t="s">
+      <c r="E33" s="2"/>
+      <c r="F33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="2" t="s">
+      <c r="G33" s="9"/>
+      <c r="H33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J33" s="8" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>